<commit_message>
3. Double check load values (Done) 4. Number of taps on transformers (Done)
</commit_message>
<xml_diff>
--- a/Outputs/CYME_Extract_UNB.xlsx
+++ b/Outputs/CYME_Extract_UNB.xlsx
@@ -89841,6 +89841,12 @@
       <c r="Q21" s="2">
         <v>100</v>
       </c>
+      <c r="S21" s="2">
+        <v>-16</v>
+      </c>
+      <c r="T21" s="2">
+        <v>16</v>
+      </c>
       <c r="U21" s="2">
         <v>10</v>
       </c>
@@ -89909,6 +89915,12 @@
       <c r="Q22" s="2">
         <v>100</v>
       </c>
+      <c r="S22" s="2">
+        <v>-8</v>
+      </c>
+      <c r="T22" s="2">
+        <v>8</v>
+      </c>
       <c r="U22" s="2">
         <v>10</v>
       </c>
@@ -89977,6 +89989,12 @@
       <c r="Q23" s="2">
         <v>100</v>
       </c>
+      <c r="S23" s="2">
+        <v>-8</v>
+      </c>
+      <c r="T23" s="2">
+        <v>8</v>
+      </c>
       <c r="U23" s="2">
         <v>10</v>
       </c>
@@ -90044,6 +90062,12 @@
       </c>
       <c r="Q24" s="2">
         <v>100</v>
+      </c>
+      <c r="S24" s="2">
+        <v>-16</v>
+      </c>
+      <c r="T24" s="2">
+        <v>16</v>
       </c>
       <c r="U24" s="2">
         <v>10</v>

</xml_diff>